<commit_message>
Change sampleUtterances to newline separation. Change delete logic to for loop with sleep. Update Dynamodb MaxCapactity to 50
</commit_message>
<xml_diff>
--- a/playground/ChatBot.xlsx
+++ b/playground/ChatBot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OrderFlowersBot" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="151">
   <si>
     <t>name</t>
   </si>
@@ -399,15 +399,6 @@
   </si>
   <si>
     <t>Type of dentist appointment to schedule</t>
-  </si>
-  <si>
-    <t>I would like to book an appointment</t>
-  </si>
-  <si>
-    <t>Book an appointment</t>
-  </si>
-  <si>
-    <t>Book a ​{AppointmentType}​</t>
   </si>
   <si>
     <t>What type of appointment would you like to schedule?</t>
@@ -475,12 +466,6 @@
     <t>FlowerType</t>
   </si>
   <si>
-    <t>I would like to order some flowers</t>
-  </si>
-  <si>
-    <t>I would like to pick up flowers</t>
-  </si>
-  <si>
     <t>Okay, I will not place your order.</t>
   </si>
   <si>
@@ -500,6 +485,15 @@
   </si>
   <si>
     <t>Types of flowers to pick up</t>
+  </si>
+  <si>
+    <t>I would like to book an appointment
+Book an appointment
+Book a ​{AppointmentType}​</t>
+  </si>
+  <si>
+    <t>I would like to pick up flowers
+I would like to order some flowers</t>
   </si>
 </sst>
 </file>
@@ -856,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -944,14 +938,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" style="4" customWidth="1"/>
+    <col min="2" max="2" width="42" style="4" customWidth="1"/>
     <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -965,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -981,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -989,18 +983,15 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>145</v>
+      <c r="B5" s="5" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1033,16 +1024,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>107</v>
@@ -1051,18 +1042,18 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>34</v>
@@ -1076,13 +1067,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>95</v>
@@ -1129,13 +1120,13 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" style="4" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="89" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -1149,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1165,7 +1156,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,21 +1164,15 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>124</v>
+      <c r="B5" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1220,16 +1205,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>107</v>
@@ -1238,18 +1223,18 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>34</v>
@@ -1263,13 +1248,13 @@
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>95</v>
@@ -1330,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,17 +1331,17 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add SNS support for new message.
</commit_message>
<xml_diff>
--- a/playground/ChatBot.xlsx
+++ b/playground/ChatBot.xlsx
@@ -20,9 +20,6 @@
     <sheet name="AppointmentTypes" sheetId="2" r:id="rId6"/>
     <sheet name="Option" sheetId="3" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
   <si>
     <t>name</t>
   </si>
@@ -381,9 +378,6 @@
   </si>
   <si>
     <t>I didn't understand you, what would you like to do?</t>
-  </si>
-  <si>
-    <t>Bot</t>
   </si>
   <si>
     <t>Bot to book a dentist appointment</t>
@@ -494,16 +488,31 @@
   <si>
     <t>I would like to pick up flowers
 I would like to order some flowers</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>cywong@vtc.edu.hk
+cy.gdoc@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -532,10 +541,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -549,8 +559,13 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -564,25 +579,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="OrderFlowersBot"/>
-      <sheetName val="OrderFlowersIntend"/>
-      <sheetName val="FlowerTypes"/>
-      <sheetName val="Option"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,7 +847,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -895,7 +891,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,10 +932,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -975,7 +971,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -983,7 +979,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -991,97 +987,103 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F9" s="4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1097,17 +1099,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Option!$B$2:$B$93</xm:f>
+          </x14:formula1>
+          <xm:sqref>D9:D11</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\cyrus\Desktop\[OrderFlowersChatbot.xlsx]Option'!#REF!</xm:f>
+            <xm:f>Option!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E8:E17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>'C:\Users\cyrus\Desktop\[OrderFlowersChatbot.xlsx]Option'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D8:D17</xm:sqref>
+          <xm:sqref>E9:E11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1117,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1156,7 +1158,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1164,7 +1166,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1172,97 +1174,105 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>150</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>127</v>
+      <c r="C9" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F9" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1273,8 +1283,11 @@
       <formula2>10</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="cywong@vtc.edu.hk"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
@@ -1282,13 +1295,13 @@
           <x14:formula1>
             <xm:f>Option!$B$2:$B$93</xm:f>
           </x14:formula1>
-          <xm:sqref>D8:D10</xm:sqref>
+          <xm:sqref>D9:D11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Option!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E8:E10</xm:sqref>
+          <xm:sqref>E9:E11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1298,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1331,22 +1344,17 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1364,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\cyrus\Desktop\[OrderFlowersChatbot.xlsx]Option'!#REF!</xm:f>
+            <xm:f>Option!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
@@ -1368,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1401,22 +1409,17 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename Intend to Intent.
</commit_message>
<xml_diff>
--- a/playground/ChatBot.xlsx
+++ b/playground/ChatBot.xlsx
@@ -9,16 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="OrderFlowersBot" sheetId="5" r:id="rId1"/>
-    <sheet name="ScheduleAppointmentBot" sheetId="1" r:id="rId2"/>
-    <sheet name="OrderFlowersIntend" sheetId="6" r:id="rId3"/>
-    <sheet name="MakeAppointmentIntend" sheetId="4" r:id="rId4"/>
-    <sheet name="FlowerTypes" sheetId="7" r:id="rId5"/>
-    <sheet name="AppointmentTypes" sheetId="2" r:id="rId6"/>
-    <sheet name="Option" sheetId="3" r:id="rId7"/>
+    <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
+    <sheet name="OrderFlowersIntent" sheetId="6" r:id="rId2"/>
+    <sheet name="MakeAppointmentIntent" sheetId="4" r:id="rId3"/>
+    <sheet name="FlowerType" sheetId="7" r:id="rId4"/>
+    <sheet name="AppointmentType" sheetId="2" r:id="rId5"/>
+    <sheet name="Option" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,13 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="151">
   <si>
     <t>valueSelectionStrategy</t>
   </si>
@@ -47,30 +40,9 @@
     <t>ORIGINAL_VALUE</t>
   </si>
   <si>
-    <t>enumerationValues</t>
-  </si>
-  <si>
-    <t>confirmationPrompt</t>
-  </si>
-  <si>
-    <t>maxAttempts</t>
-  </si>
-  <si>
-    <t>rejectionStatement</t>
-  </si>
-  <si>
-    <t>sampleUtterances</t>
-  </si>
-  <si>
-    <t>slots</t>
-  </si>
-  <si>
     <t>slotType</t>
   </si>
   <si>
-    <t>content</t>
-  </si>
-  <si>
     <t>slotConstraint</t>
   </si>
   <si>
@@ -362,25 +334,13 @@
     <t>The date to pick up the flowers</t>
   </si>
   <si>
-    <t>priority</t>
-  </si>
-  <si>
     <t>The time to pick up the flowers</t>
   </si>
   <si>
-    <t>abortStatement</t>
-  </si>
-  <si>
-    <t>clarificationPrompt</t>
-  </si>
-  <si>
     <t>Sorry, I'm not able to assist at this time</t>
   </si>
   <si>
     <t>I didn't understand you, what would you like to do?</t>
-  </si>
-  <si>
-    <t>Bot to book a dentist appointment</t>
   </si>
   <si>
     <t>cleaning</t>
@@ -427,15 +387,9 @@
     <t>{Time} is available, should I go ahead and book your appointment?</t>
   </si>
   <si>
-    <t>AppointmentTypes</t>
-  </si>
-  <si>
     <t>Intent to make appointment</t>
   </si>
   <si>
-    <t>Bot to order flowers on the behalf of a user</t>
-  </si>
-  <si>
     <t>Pick up the {FlowerType} at what time on {PickupDate}?</t>
   </si>
   <si>
@@ -449,9 +403,6 @@
   </si>
   <si>
     <t>I would like to order {FlowerType}</t>
-  </si>
-  <si>
-    <t>FlowerTypes</t>
   </si>
   <si>
     <t>What type of flowers would you like to order?</t>
@@ -490,11 +441,56 @@
 I would like to order some flowers</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>cywong@vtc.edu.hk
 cy.gdoc@gmail.com</t>
+  </si>
+  <si>
+    <t>Bot to Demo Excel Lex Bot</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Abort Statement</t>
+  </si>
+  <si>
+    <t>Clarification Prompt</t>
+  </si>
+  <si>
+    <t>Max Attempts</t>
+  </si>
+  <si>
+    <t>Confirmation Prompt</t>
+  </si>
+  <si>
+    <t>Rejection Statement</t>
+  </si>
+  <si>
+    <t>Sample Utterances</t>
+  </si>
+  <si>
+    <t>Receiver Email</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Value Selection Strategy</t>
+  </si>
+  <si>
+    <t>Possible Values</t>
   </si>
 </sst>
 </file>
@@ -852,32 +848,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -888,60 +884,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42" style="4" customWidth="1"/>
+    <col min="2" max="2" width="47" style="4" customWidth="1"/>
     <col min="3" max="3" width="55.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -952,15 +904,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -968,100 +920,98 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>141</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>142</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>9</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
@@ -1069,19 +1019,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
@@ -1117,12 +1067,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,15 +1089,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1155,102 +1105,100 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>141</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>142</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>9</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
@@ -1258,26 +1206,26 @@
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>1</formula1>
       <formula2>10</formula2>
@@ -1290,7 +1238,7 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>Option!$B$2:$B$93</xm:f>
@@ -1309,52 +1257,117 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Option!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1376,71 +1389,6 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Option!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1456,485 +1404,485 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove email hyper link.
</commit_message>
<xml_diff>
--- a/playground/ChatBot.xlsx
+++ b/playground/ChatBot.xlsx
@@ -489,7 +489,7 @@
     <t>Possible Values</t>
   </si>
   <si>
-    <t>abc@gmail.com
+    <t>abcd@abc.com
 abcd@gmail.com</t>
   </si>
 </sst>
@@ -541,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -558,6 +558,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -887,7 +890,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1075,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1134,7 @@
       <c r="A6" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1231,11 +1234,8 @@
       <formula2>10</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="cywong@vtc.edu.hk"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
Add Support for synonyms in SlotType. Refactor our parameter for JSON Encode.
</commit_message>
<xml_diff>
--- a/playground/ChatBot.xlsx
+++ b/playground/ChatBot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
@@ -17,8 +17,12 @@
     <sheet name="MakeAppointmentIntent" sheetId="4" r:id="rId3"/>
     <sheet name="FlowerType" sheetId="7" r:id="rId4"/>
     <sheet name="AppointmentType" sheetId="2" r:id="rId5"/>
-    <sheet name="Option" sheetId="3" r:id="rId6"/>
+    <sheet name="GenresType" sheetId="8" r:id="rId6"/>
+    <sheet name="Option" sheetId="3" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="slotType">Option!$B$2:$B$98</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="160">
   <si>
     <t>valueSelectionStrategy</t>
   </si>
@@ -491,6 +495,35 @@
   <si>
     <t>abcd@abc.com
 abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>comedy
+funny
+humorous</t>
+  </si>
+  <si>
+    <t>Type of Genres</t>
+  </si>
+  <si>
+    <t>adventure</t>
+  </si>
+  <si>
+    <t>documentary</t>
+  </si>
+  <si>
+    <t>AMAZON.Percentage</t>
+  </si>
+  <si>
+    <t>AMAZON.PhoneNumber</t>
+  </si>
+  <si>
+    <t>AMAZON.SpeedUnit</t>
+  </si>
+  <si>
+    <t>AMAZON.US_LAST_NAME</t>
+  </si>
+  <si>
+    <t>AMAZON.WeightUnit</t>
   </si>
 </sst>
 </file>
@@ -845,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +923,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,23 +1074,20 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>1</formula1>
       <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9:D11">
+      <formula1>slotType</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>Option!$B$2:$B$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>D9:D11</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Option!$C$2:$C$3</xm:f>
@@ -1074,9 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1228,23 +1256,20 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>1</formula1>
       <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9:D11">
+      <formula1>slotType</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>Option!$B$2:$B$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>D9:D11</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Option!$C$2:$C$3</xm:f>
@@ -1327,7 +1352,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,10 +1414,76 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Option!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1509,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>98</v>
@@ -1429,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>99</v>
@@ -1437,37 +1528,37 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1532,57 +1623,57 @@
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -1592,52 +1683,52 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
@@ -1717,27 +1808,27 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -1752,136 +1843,161 @@
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>70</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>72</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel for new slot type.
</commit_message>
<xml_diff>
--- a/playground/ChatBot.xlsx
+++ b/playground/ChatBot.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Option" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="slotType">Option!$B$2:$B$98</definedName>
+    <definedName name="slotType">Option!$B$2:$B$95</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="160">
   <si>
     <t>valueSelectionStrategy</t>
   </si>
@@ -54,18 +54,6 @@
   </si>
   <si>
     <t>AMAZON.AT_REGION</t>
-  </si>
-  <si>
-    <t>AMAZON.Actor</t>
-  </si>
-  <si>
-    <t>AMAZON.AdministrativeArea</t>
-  </si>
-  <si>
-    <t>AMAZON.AggregateRating</t>
-  </si>
-  <si>
-    <t>AMAZON.Airline</t>
   </si>
   <si>
     <t>AMAZON.Airport</t>
@@ -533,6 +521,9 @@
   </si>
   <si>
     <t>The type of appointment</t>
+  </si>
+  <si>
+    <t>AMAZON.EmailAddress</t>
   </si>
 </sst>
 </file>
@@ -899,26 +890,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -949,15 +940,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -965,31 +956,31 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B6" s="6"/>
     </row>
@@ -998,65 +989,65 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
@@ -1064,19 +1055,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
@@ -1113,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1131,15 +1122,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -1147,34 +1138,34 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1182,65 +1173,65 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
@@ -1248,19 +1239,19 @@
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F11" s="4">
         <v>3</v>
@@ -1309,15 +1300,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1325,20 +1316,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1374,15 +1365,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1390,20 +1381,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1439,15 +1430,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1455,20 +1446,20 @@
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1491,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,7 +1514,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1534,7 +1525,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1544,32 +1535,32 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1614,47 +1605,47 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
@@ -1664,27 +1655,27 @@
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -1694,37 +1685,37 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
@@ -1744,87 +1735,87 @@
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
@@ -1839,122 +1830,122 @@
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>66</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
@@ -1969,47 +1960,32 @@
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new  Built-in Slot Types.
</commit_message>
<xml_diff>
--- a/playground/ChatBot.xlsx
+++ b/playground/ChatBot.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E44BC5-6424-4829-9A72-F7146F3858FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="2700" tabRatio="639" activeTab="6"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="639" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelLexBot" sheetId="5" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="Option" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="slotType">Option!$B$2:$B$95</definedName>
+    <definedName name="slotType">Option!$B$2:$B$101</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="161">
   <si>
     <t>valueSelectionStrategy</t>
   </si>
@@ -525,11 +526,14 @@
   <si>
     <t>AMAZON.EmailAddress</t>
   </si>
+  <si>
+    <t>AMAZON.AlphaNumeric</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -875,7 +879,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -919,11 +923,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,11 +1079,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9:D11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9:D11" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>slotType</formula1>
     </dataValidation>
   </dataValidations>
@@ -1088,7 +1092,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Option!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -1101,11 +1105,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,11 +1263,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9:D11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D9:D11" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>slotType</formula1>
     </dataValidation>
   </dataValidations>
@@ -1272,7 +1276,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>Option!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -1285,7 +1289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1337,7 +1341,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Option!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1350,7 +1354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1402,7 +1406,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Option!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1415,7 +1419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1468,7 +1472,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>Option!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1481,11 +1485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>95</v>
@@ -1530,465 +1534,498 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>159</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>33</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>155</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B101">
+    <sortCondition ref="B101"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>